<commit_message>
#734 Got first test in expression-data-import-tests.js to pass.
</commit_message>
<xml_diff>
--- a/test-files/expression-data-test-sheets/expression_sheet_not_existing.xlsx
+++ b/test-files/expression-data-test-sheets/expression_sheet_not_existing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\OneDrive\GRNsight\test-files\expression-data-test-sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\Documents\GRNsight\test-files\expression-data-test-sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375C803D-1DFF-48FE-AA8D-EB178380771E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0855C3-7D96-4016-8735-6DF6CA94812F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5520" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="network" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
   <si>
     <t>ACE2</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>cols regulators/rows targets</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -1220,7 +1223,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1230,7 +1233,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>

</xml_diff>